<commit_message>
Update paired t-test: baca data dari Excel
</commit_message>
<xml_diff>
--- a/data_uji.xlsx
+++ b/data_uji.xlsx
@@ -18,10 +18,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Before</t>
+    <t>Sebelum</t>
   </si>
   <si>
-    <t>After</t>
+    <t>Sesudah</t>
   </si>
 </sst>
 </file>
@@ -377,7 +377,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>